<commit_message>
W.I.P trying to fix EmxImportServiceTest
</commit_message>
<xml_diff>
--- a/molgenis-data-mysql/src/test/resources/example.xlsx
+++ b/molgenis-data-mysql/src/test/resources/example.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="attributes" sheetId="1" r:id="rId1"/>
+    <sheet name="packages" sheetId="5" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
-    <sheet name="import_person" sheetId="3" r:id="rId3"/>
-    <sheet name="import_city" sheetId="4" r:id="rId4"/>
+    <sheet name="attributes" sheetId="1" r:id="rId3"/>
+    <sheet name="importperson" sheetId="3" r:id="rId4"/>
+    <sheet name="importcity" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -36,9 +37,6 @@
     <t>entity</t>
   </si>
   <si>
-    <t>import_person</t>
-  </si>
-  <si>
     <t>height</t>
   </si>
   <si>
@@ -63,9 +61,6 @@
     <t>birthplace</t>
   </si>
   <si>
-    <t>import_city</t>
-  </si>
-  <si>
     <t>xref</t>
   </si>
   <si>
@@ -106,6 +101,30 @@
   </si>
   <si>
     <t>john,jane</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>molgenis</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>Molgenis test importer</t>
+  </si>
+  <si>
+    <t>importcity</t>
+  </si>
+  <si>
+    <t>importperson</t>
   </si>
 </sst>
 </file>
@@ -154,8 +173,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -172,19 +197,25 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,10 +545,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -535,16 +681,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -552,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -566,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -580,57 +726,149 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D1" t="s">
         <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>179</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>179</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>180</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -643,145 +881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>179</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>179</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>180</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -798,12 +898,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "W.I.P trying to fix EmxImportServiceTest"
</commit_message>
<xml_diff>
--- a/molgenis-data-mysql/src/test/resources/example.xlsx
+++ b/molgenis-data-mysql/src/test/resources/example.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="packages" sheetId="5" r:id="rId1"/>
+    <sheet name="attributes" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
-    <sheet name="attributes" sheetId="1" r:id="rId3"/>
-    <sheet name="importperson" sheetId="3" r:id="rId4"/>
-    <sheet name="importcity" sheetId="4" r:id="rId5"/>
+    <sheet name="import_person" sheetId="3" r:id="rId3"/>
+    <sheet name="import_city" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -37,6 +36,9 @@
     <t>entity</t>
   </si>
   <si>
+    <t>import_person</t>
+  </si>
+  <si>
     <t>height</t>
   </si>
   <si>
@@ -61,6 +63,9 @@
     <t>birthplace</t>
   </si>
   <si>
+    <t>import_city</t>
+  </si>
+  <si>
     <t>xref</t>
   </si>
   <si>
@@ -101,30 +106,6 @@
   </si>
   <si>
     <t>john,jane</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>molgenis</t>
-  </si>
-  <si>
-    <t>org</t>
-  </si>
-  <si>
-    <t>package</t>
-  </si>
-  <si>
-    <t>Molgenis test importer</t>
-  </si>
-  <si>
-    <t>importcity</t>
-  </si>
-  <si>
-    <t>importperson</t>
   </si>
 </sst>
 </file>
@@ -173,14 +154,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -197,25 +172,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,50 +514,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>29</v>
+      <c r="E8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -603,10 +645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -614,42 +656,32 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -660,141 +692,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -808,24 +708,24 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>179</v>
@@ -834,15 +734,15 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
       <c r="C3">
         <v>179</v>
@@ -851,24 +751,24 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -898,12 +798,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add functionality to support self references by xref and mref entities.
</commit_message>
<xml_diff>
--- a/molgenis-data-mysql/src/test/resources/example.xlsx
+++ b/molgenis-data-mysql/src/test/resources/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -87,25 +87,28 @@
     <t>nillable</t>
   </si>
   <si>
+    <t>doe</t>
+  </si>
+  <si>
+    <t>new york</t>
+  </si>
+  <si>
+    <t>jane</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>geofrey</t>
+  </si>
+  <si>
+    <t>john,jane</t>
+  </si>
+  <si>
     <t>john</t>
   </si>
   <si>
-    <t>doe</t>
-  </si>
-  <si>
-    <t>new york</t>
-  </si>
-  <si>
-    <t>jane</t>
-  </si>
-  <si>
-    <t>washington</t>
-  </si>
-  <si>
-    <t>geofrey</t>
-  </si>
-  <si>
-    <t>john,jane</t>
+    <t>parent</t>
   </si>
 </sst>
 </file>
@@ -118,6 +121,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -154,8 +158,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -172,19 +190,33 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -633,8 +665,23 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -654,6 +701,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -692,15 +740,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -719,13 +767,16 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>179</v>
@@ -734,15 +785,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>179</v>
@@ -751,28 +805,35 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>180</v>
       </c>
       <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -798,12 +859,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>